<commit_message>
v0.2 changes Updated: JSON-Server (Posts API) Testcases.xlsx
</commit_message>
<xml_diff>
--- a/JSON-Server (Posts API) Testcases.xlsx
+++ b/JSON-Server (Posts API) Testcases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Get all the available posts</t>
-  </si>
-  <si>
-    <t>JSON</t>
   </si>
   <si>
     <t>Description</t>
@@ -364,6 +361,18 @@
       </rPr>
       <t>npm -g install json-server</t>
     </r>
+  </si>
+  <si>
+    <t>DELTE</t>
+  </si>
+  <si>
+    <t>Try to Delete the post without passing any id</t>
+  </si>
+  <si>
+    <t>Response Content-type</t>
+  </si>
+  <si>
+    <t>application/json</t>
   </si>
 </sst>
 </file>
@@ -472,12 +481,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -497,6 +500,12 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,9 +514,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF5050"/>
       <color rgb="FFFE84BB"/>
       <color rgb="FFFC7CCE"/>
-      <color rgb="FFFF5050"/>
       <color rgb="FF66CCFF"/>
       <color rgb="FF0099FF"/>
     </mruColors>
@@ -786,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:I5"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,110 +809,119 @@
     <col min="4" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="J6" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -913,562 +931,667 @@
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="6">
+        <v>200</v>
+      </c>
+      <c r="J7" s="6">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <f xml:space="preserve"> A7+1</f>
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I8" s="6">
         <v>200</v>
       </c>
-      <c r="I7" s="6">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="J8" s="6">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <f t="shared" ref="A9:A26" si="0" xml:space="preserve"> A8+1</f>
+        <v>3</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="6">
-        <v>200</v>
-      </c>
-      <c r="I8" s="6">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>3</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="6">
+        <v>404</v>
+      </c>
+      <c r="J9" s="7">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="H9" s="6">
-        <v>404</v>
-      </c>
-      <c r="I9" s="7">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>4</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="6">
+        <v>201</v>
+      </c>
+      <c r="J10" s="6">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="6">
-        <v>201</v>
-      </c>
-      <c r="I10" s="6">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>5</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>15</v>
+      <c r="B11" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>201</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J11" s="6">
         <v>676</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>15</v>
+      <c r="B12" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="6">
+      <c r="I12" s="6">
         <v>500</v>
       </c>
-      <c r="I12" s="6">
+      <c r="J12" s="6">
         <v>706</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>15</v>
+      <c r="B13" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="6">
+        <v>400</v>
+      </c>
+      <c r="J13" s="6">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="6">
+        <v>200</v>
+      </c>
+      <c r="J14" s="6">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="6">
+        <v>404</v>
+      </c>
+      <c r="J15" s="6">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="6">
+        <v>200</v>
+      </c>
+      <c r="J16" s="6">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="6">
+        <v>200</v>
+      </c>
+      <c r="J17" s="6">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="6">
+      <c r="E18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="6">
         <v>400</v>
       </c>
-      <c r="I13" s="6">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>8</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="J18" s="6">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="6">
+        <v>200</v>
+      </c>
+      <c r="J19" s="6">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="6">
+        <v>404</v>
+      </c>
+      <c r="J20" s="6">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="6">
+        <v>200</v>
+      </c>
+      <c r="J21" s="6">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="6">
+      <c r="B22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="6">
         <v>200</v>
       </c>
-      <c r="I14" s="6">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>9</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="J22" s="6">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="6">
+        <v>400</v>
+      </c>
+      <c r="J23" s="6">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="6">
+        <v>200</v>
+      </c>
+      <c r="J24" s="6">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="6">
         <v>404</v>
       </c>
-      <c r="I15" s="6">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>10</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="6">
-        <v>200</v>
-      </c>
-      <c r="I16" s="6">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>11</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="6">
-        <v>200</v>
-      </c>
-      <c r="I17" s="6">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>12</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="6">
-        <v>400</v>
-      </c>
-      <c r="I18" s="6">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="J25" s="6">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="6">
-        <v>200</v>
-      </c>
-      <c r="I19" s="6">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>14</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="6">
+      <c r="I26" s="6">
         <v>404</v>
       </c>
-      <c r="I20" s="6">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>15</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="6">
-        <v>200</v>
-      </c>
-      <c r="I21" s="6">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>16</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="6">
-        <v>200</v>
-      </c>
-      <c r="I22" s="6">
+      <c r="J26" s="6">
         <v>526</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>17</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H23" s="6">
-        <v>400</v>
-      </c>
-      <c r="I23" s="6">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>18</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="6">
-        <v>200</v>
-      </c>
-      <c r="I24" s="6">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>19</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="6">
-        <v>404</v>
-      </c>
-      <c r="I25" s="6">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -1488,11 +1611,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>